<commit_message>
Update README with project details, add requirements file, and include new output files. Update image files and remove unnecessary cache files.
</commit_message>
<xml_diff>
--- a/evaluation/evaluation_results.xlsx
+++ b/evaluation/evaluation_results.xlsx
@@ -454,7 +454,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9783236994219653</v>
+        <v>0.7596339113680154</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9790086499094979</v>
+        <v>0.847297768612078</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9783236994219653</v>
+        <v>0.7596339113680154</v>
       </c>
     </row>
     <row r="5">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9783381279251664</v>
+        <v>0.7549191201777731</v>
       </c>
     </row>
   </sheetData>
@@ -540,13 +540,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.9223300970873787</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9900990099009901</v>
+        <v>0.9405940594059405</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9950248756218906</v>
+        <v>0.9313725490196079</v>
       </c>
       <c r="E2" t="n">
         <v>101</v>
@@ -559,13 +559,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9932885906040269</v>
+        <v>0.8690476190476191</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9932885906040269</v>
+        <v>0.9798657718120806</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9932885906040269</v>
+        <v>0.9211356466876972</v>
       </c>
       <c r="E3" t="n">
         <v>149</v>
@@ -578,13 +578,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9900990099009901</v>
+        <v>0.7518796992481203</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9950248756218906</v>
+        <v>0.8583690987124464</v>
       </c>
       <c r="E4" t="n">
         <v>100</v>
@@ -597,13 +597,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9795918367346939</v>
+        <v>0.9047619047619048</v>
       </c>
       <c r="C5" t="n">
-        <v>0.96</v>
+        <v>0.76</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9696969696969697</v>
+        <v>0.8260869565217391</v>
       </c>
       <c r="E5" t="n">
         <v>100</v>
@@ -616,13 +616,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9375</v>
+        <v>0.5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.967741935483871</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="E6" t="n">
         <v>16</v>
@@ -635,13 +635,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9858490566037735</v>
+        <v>0.9904761904761905</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9766355140186916</v>
+        <v>0.485981308411215</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9812206572769953</v>
+        <v>0.6520376175548589</v>
       </c>
       <c r="E7" t="n">
         <v>214</v>
@@ -654,13 +654,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9587628865979382</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.93</v>
+        <v>0.06</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9441624365482234</v>
+        <v>0.1132075471698113</v>
       </c>
       <c r="E8" t="n">
         <v>100</v>
@@ -673,13 +673,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9777777777777777</v>
+        <v>0.8019323671497585</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.8645833333333334</v>
       </c>
       <c r="D9" t="n">
-        <v>0.946236559139785</v>
+        <v>0.8320802005012531</v>
       </c>
       <c r="E9" t="n">
         <v>192</v>
@@ -692,13 +692,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8878504672897196</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9895833333333334</v>
+        <v>0.90625</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9359605911330049</v>
+        <v>0.725</v>
       </c>
       <c r="E10" t="n">
         <v>96</v>
@@ -711,13 +711,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9672131147540983</v>
+        <v>0.5342019543973942</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9943820224719101</v>
+        <v>0.9213483146067416</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9806094182825484</v>
+        <v>0.6762886597938145</v>
       </c>
       <c r="E11" t="n">
         <v>178</v>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9940119760479041</v>
+        <v>0.8675496688741722</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9880952380952381</v>
+        <v>0.7797619047619048</v>
       </c>
       <c r="D12" t="n">
-        <v>0.991044776119403</v>
+        <v>0.8213166144200627</v>
       </c>
       <c r="E12" t="n">
         <v>168</v>
@@ -749,13 +749,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.8429752066115702</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9929577464788732</v>
+        <v>0.7183098591549296</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9657534246575342</v>
+        <v>0.7756653992395437</v>
       </c>
       <c r="E13" t="n">
         <v>142</v>
@@ -768,13 +768,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.996875</v>
+        <v>0.9949748743718593</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9906832298136646</v>
+        <v>0.6149068322981367</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9937694704049844</v>
+        <v>0.7600767754318618</v>
       </c>
       <c r="E14" t="n">
         <v>322</v>
@@ -787,13 +787,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>0.2303030303030303</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9473684210526315</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0.972972972972973</v>
+        <v>0.374384236453202</v>
       </c>
       <c r="E15" t="n">
         <v>38</v>
@@ -806,13 +806,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9937888198757764</v>
+        <v>0.9017341040462428</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0.975</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9968847352024922</v>
+        <v>0.9369369369369369</v>
       </c>
       <c r="E16" t="n">
         <v>160</v>
@@ -921,13 +921,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -976,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -985,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1077,16 +1077,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1098,13 +1098,13 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -1132,16 +1132,16 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -1181,46 +1181,46 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>209</v>
+        <v>104</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -1233,16 +1233,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1251,28 +1251,28 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K8" t="n">
+        <v>44</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
         <v>2</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>4</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
@@ -1288,13 +1288,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1303,31 +1303,31 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="J9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K9" t="n">
+        <v>5</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
         <v>2</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -1358,25 +1358,25 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
@@ -1392,10 +1392,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1404,19 +1404,19 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
@@ -1444,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -1471,19 +1471,19 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="M12" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -1493,13 +1493,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1517,16 +1517,16 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M13" t="n">
-        <v>141</v>
+        <v>102</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -1535,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -1560,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1569,22 +1569,22 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" t="n">
-        <v>319</v>
+        <v>198</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
@@ -1621,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -1636,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1688,10 +1688,10 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" t="n">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove unused image file and update README to streamline dependency installation. Add openpyxl to requirements.txt for enhanced functionality.
</commit_message>
<xml_diff>
--- a/evaluation/evaluation_results.xlsx
+++ b/evaluation/evaluation_results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Class Metrics" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Confusion Matrix" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Class Metrics" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Confusion Matrix" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -454,7 +454,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7596339113680154</v>
+        <v>0.9961464354527938</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.847297768612078</v>
+        <v>0.9961679096987319</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7596339113680154</v>
+        <v>0.9961464354527938</v>
       </c>
     </row>
     <row r="5">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7549191201777731</v>
+        <v>0.9961458503010788</v>
       </c>
     </row>
   </sheetData>
@@ -540,13 +540,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9223300970873787</v>
+        <v>0.9901960784313726</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9405940594059405</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9313725490196079</v>
+        <v>0.9950738916256158</v>
       </c>
       <c r="E2" t="n">
         <v>101</v>
@@ -559,13 +559,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8690476190476191</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9798657718120806</v>
+        <v>0.9932885906040269</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9211356466876972</v>
+        <v>0.9966329966329966</v>
       </c>
       <c r="E3" t="n">
         <v>149</v>
@@ -578,13 +578,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7518796992481203</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8583690987124464</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>100</v>
@@ -597,13 +597,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9047619047619048</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.76</v>
+        <v>0.98</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8260869565217391</v>
+        <v>0.9898989898989899</v>
       </c>
       <c r="E5" t="n">
         <v>100</v>
@@ -616,13 +616,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6153846153846154</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>16</v>
@@ -635,13 +635,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9904761904761905</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.485981308411215</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6520376175548589</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>214</v>
@@ -657,10 +657,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.06</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1132075471698113</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
         <v>100</v>
@@ -673,13 +673,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8019323671497585</v>
+        <v>0.9896373056994818</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8645833333333334</v>
+        <v>0.9947916666666666</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8320802005012531</v>
+        <v>0.9922077922077922</v>
       </c>
       <c r="E9" t="n">
         <v>192</v>
@@ -692,13 +692,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6041666666666666</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0.90625</v>
+        <v>0.9895833333333334</v>
       </c>
       <c r="D10" t="n">
-        <v>0.725</v>
+        <v>0.9947643979057592</v>
       </c>
       <c r="E10" t="n">
         <v>96</v>
@@ -711,13 +711,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5342019543973942</v>
+        <v>0.994413407821229</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9213483146067416</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6762886597938145</v>
+        <v>0.9971988795518207</v>
       </c>
       <c r="E11" t="n">
         <v>178</v>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.8675496688741722</v>
+        <v>0.9881656804733728</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7797619047619048</v>
+        <v>0.9940476190476191</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8213166144200627</v>
+        <v>0.9910979228486647</v>
       </c>
       <c r="E12" t="n">
         <v>168</v>
@@ -749,13 +749,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.8429752066115702</v>
+        <v>0.993006993006993</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7183098591549296</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7756653992395437</v>
+        <v>0.9964912280701754</v>
       </c>
       <c r="E13" t="n">
         <v>142</v>
@@ -768,13 +768,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9949748743718593</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6149068322981367</v>
+        <v>0.9968944099378882</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7600767754318618</v>
+        <v>0.9984447900466563</v>
       </c>
       <c r="E14" t="n">
         <v>322</v>
@@ -787,13 +787,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.2303030303030303</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0.374384236453202</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
         <v>38</v>
@@ -806,13 +806,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9017341040462428</v>
+        <v>0.99375</v>
       </c>
       <c r="C16" t="n">
-        <v>0.975</v>
+        <v>0.99375</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9369369369369369</v>
+        <v>0.99375</v>
       </c>
       <c r="E16" t="n">
         <v>160</v>
@@ -921,13 +921,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -973,10 +973,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -985,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1000,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -1077,34 +1077,34 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>98</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
         <v>2</v>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E5" t="n">
-        <v>76</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>13</v>
-      </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -1132,16 +1132,16 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1181,46 +1181,46 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -1233,16 +1233,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1251,16 +1251,16 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="I8" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -1272,7 +1272,7 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
@@ -1288,13 +1288,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1306,13 +1306,13 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="J9" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
@@ -1321,13 +1321,13 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -1358,25 +1358,25 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
@@ -1392,10 +1392,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1404,19 +1404,19 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
@@ -1444,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -1465,25 +1465,25 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="M12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1493,13 +1493,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1517,16 +1517,16 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -1535,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -1569,22 +1569,22 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>198</v>
+        <v>321</v>
       </c>
       <c r="O14" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" t="n">
         <v>0</v>
@@ -1688,10 +1688,10 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>